<commit_message>
Actualizacion con pendientes 240627
</commit_message>
<xml_diff>
--- a/Datos_ent/Base.xlsx
+++ b/Datos_ent/Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bancolombia-my.sharepoint.com/personal/arygonza_bancolombia_com_co/Documents/Bancolombia_ARGO/Bancolombia_Argo_2023/Personales/Econometria_Uext/VAR_Models/Datos_ent/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\repos\VAR_Models\Datos_ent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{64048535-1783-43CD-A5F6-14EF31E638C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8558B70-DA05-4D8B-9929-7F186544ACAE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6FB0DD-2B09-4126-AB48-7D65594F2586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{F7DE5675-7431-4D40-AC4D-5D3792C506F0}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{F7DE5675-7431-4D40-AC4D-5D3792C506F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Fuente:</t>
   </si>
@@ -61,13 +61,16 @@
   <si>
     <t>fecha</t>
   </si>
+  <si>
+    <t>EMBI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -130,7 +133,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -155,9 +158,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -195,7 +198,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -301,7 +304,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -443,7 +446,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -451,15 +454,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06AA51F-FD66-422B-8077-68ED66061B9A}">
-  <dimension ref="A1:D214"/>
+  <dimension ref="A1:E224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="D224" sqref="D224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -486,22 +489,25 @@
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>38718</v>
       </c>
       <c r="B4" s="3">
-        <v>2271.4909523809524</v>
+        <v>2271.9709090909096</v>
       </c>
       <c r="C4" s="4">
         <v>62.99</v>
       </c>
       <c r="D4" s="4">
-        <v>100.00000454545453</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89.121818181818185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>38749</v>
       </c>
@@ -512,10 +518,10 @@
         <v>60.21</v>
       </c>
       <c r="D5" s="4">
-        <v>100.21117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.36699999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>38777</v>
       </c>
@@ -526,10 +532,10 @@
         <v>62.06</v>
       </c>
       <c r="D6" s="4">
-        <v>100.42808695652175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89.966956521739135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>38808</v>
       </c>
@@ -540,10 +546,10 @@
         <v>70.260000000000005</v>
       </c>
       <c r="D7" s="4">
-        <v>99.743480000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>88.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>38838</v>
       </c>
@@ -554,10 +560,10 @@
         <v>69.78</v>
       </c>
       <c r="D8" s="4">
-        <v>97.511773913043484</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84.874782608695654</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>38869</v>
       </c>
@@ -568,10 +574,10 @@
         <v>68.56</v>
       </c>
       <c r="D9" s="4">
-        <v>98.692722727272752</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85.765909090909091</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>38899</v>
       </c>
@@ -582,10 +588,10 @@
         <v>73.67</v>
       </c>
       <c r="D10" s="4">
-        <v>98.438714285714298</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85.859047619047629</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>38930</v>
       </c>
@@ -596,10 +602,10 @@
         <v>73.23</v>
       </c>
       <c r="D11" s="4">
-        <v>97.713765217391327</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85.045217391304334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>38961</v>
       </c>
@@ -610,10 +616,10 @@
         <v>61.96</v>
       </c>
       <c r="D12" s="4">
-        <v>97.981361904761911</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85.572857142857146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>38991</v>
       </c>
@@ -624,10 +630,10 @@
         <v>57.81</v>
       </c>
       <c r="D13" s="4">
-        <v>98.315654545454535</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86.342727272727259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>39022</v>
       </c>
@@ -638,10 +644,10 @@
         <v>58.76</v>
       </c>
       <c r="D14" s="4">
-        <v>97.51328181818181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84.844545454545468</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>39052</v>
       </c>
@@ -652,10 +658,10 @@
         <v>62.47</v>
       </c>
       <c r="D15" s="4">
-        <v>96.795071428571418</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83.38333333333334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>39083</v>
       </c>
@@ -666,10 +672,10 @@
         <v>53.68</v>
       </c>
       <c r="D16" s="4">
-        <v>97.833777272727275</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84.745217391304337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>39114</v>
       </c>
@@ -680,10 +686,10 @@
         <v>57.56</v>
       </c>
       <c r="D17" s="4">
-        <v>97.476425000000006</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84.390500000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>39142</v>
       </c>
@@ -694,10 +700,10 @@
         <v>62.05</v>
       </c>
       <c r="D18" s="4">
-        <v>97.011754545454536</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83.484090909090909</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>39173</v>
       </c>
@@ -708,10 +714,10 @@
         <v>67.489999999999995</v>
       </c>
       <c r="D19" s="4">
-        <v>95.632199999999969</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.190142857142874</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>39203</v>
       </c>
@@ -722,10 +728,10 @@
         <v>67.209999999999994</v>
       </c>
       <c r="D20" s="4">
-        <v>94.722547826086966</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.118913043478244</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>39234</v>
       </c>
@@ -736,10 +742,10 @@
         <v>71.05</v>
       </c>
       <c r="D21" s="4">
-        <v>94.444909523809514</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.466761904761924</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>39264</v>
       </c>
@@ -750,10 +756,10 @@
         <v>76.930000000000007</v>
       </c>
       <c r="D22" s="4">
-        <v>93.205913636363633</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.808909090909097</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>39295</v>
       </c>
@@ -764,10 +770,10 @@
         <v>70.760000000000005</v>
       </c>
       <c r="D23" s="4">
-        <v>93.760295652173895</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.935173913043485</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>39326</v>
       </c>
@@ -778,10 +784,10 @@
         <v>77.17</v>
       </c>
       <c r="D24" s="4">
-        <v>92.436595000000011</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.37684999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>39356</v>
       </c>
@@ -792,10 +798,10 @@
         <v>82.34</v>
       </c>
       <c r="D25" s="4">
-        <v>90.400178260869581</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77.847347826086946</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>39387</v>
       </c>
@@ -806,10 +812,10 @@
         <v>92.41</v>
       </c>
       <c r="D26" s="4">
-        <v>89.052995454545439</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75.641227272727264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>39417</v>
       </c>
@@ -820,10 +826,10 @@
         <v>90.93</v>
       </c>
       <c r="D27" s="4">
-        <v>90.004957142857137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76.803238095238115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>39448</v>
       </c>
@@ -834,10 +840,10 @@
         <v>92.18</v>
       </c>
       <c r="D28" s="4">
-        <v>89.397117391304363</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75.981695652173897</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>39479</v>
       </c>
@@ -848,10 +854,10 @@
         <v>94.99</v>
       </c>
       <c r="D29" s="4">
-        <v>88.643438095238082</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75.698380952380944</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>39508</v>
       </c>
@@ -862,10 +868,10 @@
         <v>103.64</v>
       </c>
       <c r="D30" s="4">
-        <v>86.83986666666668</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72.467476190476205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>39539</v>
       </c>
@@ -876,10 +882,10 @@
         <v>109.07</v>
       </c>
       <c r="D31" s="4">
-        <v>86.547536363636368</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72.116545454545445</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>39569</v>
       </c>
@@ -890,10 +896,10 @@
         <v>122.8</v>
       </c>
       <c r="D32" s="4">
-        <v>86.824463636363646</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72.86572727272727</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>39600</v>
       </c>
@@ -904,10 +910,10 @@
         <v>132.32</v>
       </c>
       <c r="D33" s="4">
-        <v>87.072804761904777</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73.179999999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>39630</v>
       </c>
@@ -918,10 +924,10 @@
         <v>132.72</v>
       </c>
       <c r="D34" s="4">
-        <v>86.453756521739137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72.545695652173876</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>39661</v>
       </c>
@@ -932,10 +938,10 @@
         <v>113.24</v>
       </c>
       <c r="D35" s="4">
-        <v>88.94499523809526</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76.060904761904766</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>39692</v>
       </c>
@@ -946,10 +952,10 @@
         <v>97.23</v>
       </c>
       <c r="D36" s="4">
-        <v>91.265109090909107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78.223090909090914</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>39722</v>
       </c>
@@ -960,10 +966,10 @@
         <v>71.58</v>
       </c>
       <c r="D37" s="4">
-        <v>98.039999999999978</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83.111956521739117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>39753</v>
       </c>
@@ -974,10 +980,10 @@
         <v>52.45</v>
       </c>
       <c r="D38" s="4">
-        <v>100.76666</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86.391449999999992</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>39783</v>
       </c>
@@ -988,10 +994,10 @@
         <v>39.950000000000003</v>
       </c>
       <c r="D39" s="4">
-        <v>99.662247826086954</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.973434782608706</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39814</v>
       </c>
@@ -1002,10 +1008,10 @@
         <v>43.44</v>
       </c>
       <c r="D40" s="4">
-        <v>100.35208421052631</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83.964500000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>39845</v>
       </c>
@@ -1016,10 +1022,10 @@
         <v>43.32</v>
       </c>
       <c r="D41" s="4">
-        <v>102.97372631578946</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86.540400000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>39873</v>
       </c>
@@ -1030,10 +1036,10 @@
         <v>46.54</v>
       </c>
       <c r="D42" s="4">
-        <v>103.43974545454545</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86.410636363636343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>39904</v>
       </c>
@@ -1044,10 +1050,10 @@
         <v>50.18</v>
       </c>
       <c r="D43" s="4">
-        <v>100.71618636363637</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85.254909090909095</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>39934</v>
       </c>
@@ -1058,10 +1064,10 @@
         <v>57.3</v>
       </c>
       <c r="D44" s="4">
-        <v>97.551880000000011</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.035428571428582</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>39965</v>
       </c>
@@ -1072,10 +1078,10 @@
         <v>68.61</v>
       </c>
       <c r="D45" s="4">
-        <v>96.042618181818213</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.116636363636374</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>39995</v>
       </c>
@@ -1086,10 +1092,10 @@
         <v>64.44</v>
       </c>
       <c r="D46" s="4">
-        <v>95.660559090909061</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.526347826086948</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>40026</v>
       </c>
@@ -1100,10 +1106,10 @@
         <v>72.510000000000005</v>
       </c>
       <c r="D47" s="4">
-        <v>94.373042857142863</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78.447857142857146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>40057</v>
       </c>
@@ -1114,10 +1120,10 @@
         <v>67.650000000000006</v>
       </c>
       <c r="D48" s="4">
-        <v>93.663800000000023</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77.053090909090898</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>40087</v>
       </c>
@@ -1128,10 +1134,10 @@
         <v>72.77</v>
       </c>
       <c r="D49" s="4">
-        <v>92.259761904761888</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76.010772727272723</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>40118</v>
       </c>
@@ -1142,10 +1148,10 @@
         <v>76.66</v>
       </c>
       <c r="D50" s="4">
-        <v>91.799610526315774</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75.307619047619056</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>40148</v>
       </c>
@@ -1156,10 +1162,10 @@
         <v>74.459999999999994</v>
       </c>
       <c r="D51" s="4">
-        <v>92.258619047619035</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76.827739130434765</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>40179</v>
       </c>
@@ -1170,10 +1176,10 @@
         <v>76.17</v>
       </c>
       <c r="D52" s="4">
-        <v>92.440300000000008</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77.804904761904751</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>40210</v>
       </c>
@@ -1184,10 +1190,10 @@
         <v>73.75</v>
       </c>
       <c r="D53" s="4">
-        <v>93.886679999999998</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.164600000000007</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>40238</v>
       </c>
@@ -1198,10 +1204,10 @@
         <v>78.83</v>
       </c>
       <c r="D54" s="4">
-        <v>93.149878260869613</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.671608695652168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>40269</v>
       </c>
@@ -1212,10 +1218,10 @@
         <v>84.82</v>
       </c>
       <c r="D55" s="4">
-        <v>92.639086363636366</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81.235954545454547</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>40299</v>
       </c>
@@ -1226,10 +1232,10 @@
         <v>75.95</v>
       </c>
       <c r="D56" s="4">
-        <v>95.530640000000005</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85.419095238095252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>40330</v>
       </c>
@@ -1240,10 +1246,10 @@
         <v>74.760000000000005</v>
       </c>
       <c r="D57" s="4">
-        <v>96.060627272727288</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86.575454545454576</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>40360</v>
       </c>
@@ -1254,10 +1260,10 @@
         <v>75.58</v>
       </c>
       <c r="D58" s="4">
-        <v>94.454690476190464</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83.140045454545458</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>40391</v>
       </c>
@@ -1268,10 +1274,10 @@
         <v>77.040000000000006</v>
       </c>
       <c r="D59" s="4">
-        <v>93.682231818181833</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.148863636363615</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>40422</v>
       </c>
@@ -1282,10 +1288,10 @@
         <v>77.84</v>
       </c>
       <c r="D60" s="4">
-        <v>92.762595238095244</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81.081818181818178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>40452</v>
       </c>
@@ -1296,10 +1302,10 @@
         <v>82.67</v>
       </c>
       <c r="D61" s="4">
-        <v>90.229119999999995</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77.459952380952387</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>40483</v>
       </c>
@@ -1310,10 +1316,10 @@
         <v>85.28</v>
       </c>
       <c r="D62" s="4">
-        <v>90.509535000000014</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78.443136363636356</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>40513</v>
       </c>
@@ -1324,10 +1330,10 @@
         <v>91.45</v>
       </c>
       <c r="D63" s="4">
-        <v>91.183471428571437</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.067999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>40544</v>
       </c>
@@ -1338,10 +1344,10 @@
         <v>96.52</v>
       </c>
       <c r="D64" s="4">
-        <v>90.111219999999989</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.155380952380966</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>40575</v>
       </c>
@@ -1352,10 +1358,10 @@
         <v>103.72</v>
       </c>
       <c r="D65" s="4">
-        <v>89.396689473684233</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77.777600000000007</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>40603</v>
       </c>
@@ -1366,10 +1372,10 @@
         <v>114.64</v>
       </c>
       <c r="D66" s="4">
-        <v>88.487226086956511</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76.28765217391306</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>40634</v>
       </c>
@@ -1380,10 +1386,10 @@
         <v>123.26</v>
       </c>
       <c r="D67" s="4">
-        <v>86.921366666666643</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74.689761904761909</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>40664</v>
       </c>
@@ -1394,10 +1400,10 @@
         <v>114.99</v>
       </c>
       <c r="D68" s="4">
-        <v>86.946404761904759</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74.943090909090913</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>40695</v>
       </c>
@@ -1408,10 +1414,10 @@
         <v>113.83</v>
       </c>
       <c r="D69" s="4">
-        <v>86.941254545454569</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74.694636363636349</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>40725</v>
       </c>
@@ -1422,10 +1428,10 @@
         <v>116.97</v>
       </c>
       <c r="D70" s="4">
-        <v>86.317804999999993</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74.733999999999995</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>40756</v>
       </c>
@@ -1436,10 +1442,10 @@
         <v>110.22</v>
       </c>
       <c r="D71" s="4">
-        <v>86.898243478260866</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74.238565217391297</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>40787</v>
       </c>
@@ -1450,10 +1456,10 @@
         <v>112.83</v>
       </c>
       <c r="D72" s="4">
-        <v>89.72526666666667</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76.915454545454566</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>40817</v>
       </c>
@@ -1464,10 +1470,10 @@
         <v>109.55</v>
       </c>
       <c r="D73" s="4">
-        <v>90.609844999999993</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77.155904761904765</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>40848</v>
       </c>
@@ -1478,10 +1484,10 @@
         <v>110.77</v>
       </c>
       <c r="D74" s="4">
-        <v>91.264880000000019</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77.957499999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>40878</v>
       </c>
@@ -1492,10 +1498,10 @@
         <v>107.87</v>
       </c>
       <c r="D75" s="4">
-        <v>92.205590476190494</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.629500000000007</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>40909</v>
       </c>
@@ -1506,10 +1512,10 @@
         <v>110.69</v>
       </c>
       <c r="D76" s="4">
-        <v>91.646265</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.333045454545427</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>40940</v>
       </c>
@@ -1520,10 +1526,10 @@
         <v>119.33</v>
       </c>
       <c r="D77" s="4">
-        <v>89.96050000000001</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78.953000000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>40969</v>
       </c>
@@ -1534,10 +1540,10 @@
         <v>125.45</v>
       </c>
       <c r="D78" s="4">
-        <v>90.511213636363649</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.558909090909083</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>41000</v>
       </c>
@@ -1548,10 +1554,10 @@
         <v>119.75</v>
       </c>
       <c r="D79" s="4">
-        <v>90.815609523809528</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.429523809523815</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>41030</v>
       </c>
@@ -1562,10 +1568,10 @@
         <v>110.34</v>
       </c>
       <c r="D80" s="4">
-        <v>92.49278636363637</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.989086956521746</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>41061</v>
       </c>
@@ -1576,10 +1582,10 @@
         <v>95.16</v>
       </c>
       <c r="D81" s="4">
-        <v>93.880866666666662</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.244904761904778</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>41091</v>
       </c>
@@ -1590,10 +1596,10 @@
         <v>102.62</v>
       </c>
       <c r="D82" s="4">
-        <v>93.406166666666664</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83.022772727272724</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>41122</v>
       </c>
@@ -1604,10 +1610,10 @@
         <v>113.36</v>
       </c>
       <c r="D83" s="4">
-        <v>92.528265217391294</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.158608695652177</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>41153</v>
       </c>
@@ -1618,10 +1624,10 @@
         <v>112.86</v>
       </c>
       <c r="D84" s="4">
-        <v>90.980199999999996</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.874650000000003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>41183</v>
       </c>
@@ -1632,10 +1638,10 @@
         <v>111.71</v>
       </c>
       <c r="D85" s="4">
-        <v>90.756630000000001</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.737391304347824</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>41214</v>
       </c>
@@ -1646,10 +1652,10 @@
         <v>109.06</v>
       </c>
       <c r="D86" s="4">
-        <v>91.47508000000002</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.6965</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>41244</v>
       </c>
@@ -1660,10 +1666,10 @@
         <v>109.49</v>
       </c>
       <c r="D87" s="4">
-        <v>90.880390000000006</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.748857142857162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>41275</v>
       </c>
@@ -1674,10 +1680,10 @@
         <v>112.96</v>
       </c>
       <c r="D88" s="4">
-        <v>90.825514285714291</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.871173913043492</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>41306</v>
       </c>
@@ -1688,10 +1694,10 @@
         <v>116.05</v>
       </c>
       <c r="D89" s="4">
-        <v>91.550873684210544</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.602400000000017</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>41334</v>
       </c>
@@ -1702,10 +1708,10 @@
         <v>108.47</v>
       </c>
       <c r="D90" s="4">
-        <v>92.413179999999997</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.641190476190488</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>41365</v>
       </c>
@@ -1716,10 +1722,10 @@
         <v>102.25</v>
       </c>
       <c r="D91" s="4">
-        <v>92.047822727272717</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.523454545454541</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>41395</v>
       </c>
@@ -1730,10 +1736,10 @@
         <v>102.56</v>
       </c>
       <c r="D92" s="4">
-        <v>92.5289681818182</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83.21582608695654</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>41426</v>
       </c>
@@ -1744,10 +1750,10 @@
         <v>102.92</v>
       </c>
       <c r="D93" s="4">
-        <v>93.283614999999983</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81.873699999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>41456</v>
       </c>
@@ -1758,10 +1764,10 @@
         <v>107.93</v>
       </c>
       <c r="D94" s="4">
-        <v>93.872386363636366</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.816173913043471</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>41487</v>
       </c>
@@ -1772,10 +1778,10 @@
         <v>111.28</v>
       </c>
       <c r="D95" s="4">
-        <v>93.714886363636367</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81.481590909090926</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>41518</v>
       </c>
@@ -1786,10 +1792,10 @@
         <v>111.6</v>
       </c>
       <c r="D96" s="4">
-        <v>93.470564999999993</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81.206095238095259</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>41548</v>
       </c>
@@ -1800,10 +1806,10 @@
         <v>109.08</v>
       </c>
       <c r="D97" s="4">
-        <v>92.499268181818195</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.871217391304342</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>41579</v>
       </c>
@@ -1814,10 +1820,10 @@
         <v>107.79</v>
       </c>
       <c r="D98" s="4">
-        <v>93.373668421052614</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.846190476190515</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>41609</v>
       </c>
@@ -1828,10 +1834,10 @@
         <v>110.76</v>
       </c>
       <c r="D99" s="4">
-        <v>93.534019999999998</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.324090909090913</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>41640</v>
       </c>
@@ -1842,10 +1848,10 @@
         <v>108.12</v>
       </c>
       <c r="D100" s="4">
-        <v>94.464747619047628</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.797478260869553</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>41671</v>
       </c>
@@ -1856,10 +1862,10 @@
         <v>108.9</v>
       </c>
       <c r="D101" s="4">
-        <v>94.645582352941176</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.437300000000022</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>41699</v>
       </c>
@@ -1870,10 +1876,10 @@
         <v>107.48</v>
       </c>
       <c r="D102" s="4">
-        <v>94.440821052631591</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.871523809523808</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>41730</v>
       </c>
@@ -1884,10 +1890,10 @@
         <v>107.76</v>
       </c>
       <c r="D103" s="4">
-        <v>93.995550000000009</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.850863636363627</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>41760</v>
       </c>
@@ -1898,10 +1904,10 @@
         <v>109.54</v>
       </c>
       <c r="D104" s="4">
-        <v>93.67002857142856</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.96390909090907</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>41791</v>
       </c>
@@ -1912,10 +1918,10 @@
         <v>111.8</v>
       </c>
       <c r="D105" s="4">
-        <v>93.827404761904759</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.440238095238101</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>41821</v>
       </c>
@@ -1926,10 +1932,10 @@
         <v>106.77</v>
       </c>
       <c r="D106" s="4">
-        <v>93.603859090909069</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.535391304347826</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>41852</v>
       </c>
@@ -1940,10 +1946,10 @@
         <v>101.61</v>
       </c>
       <c r="D107" s="4">
-        <v>94.580809523809535</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81.856238095238112</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>41883</v>
       </c>
@@ -1954,10 +1960,10 @@
         <v>97.09</v>
       </c>
       <c r="D108" s="4">
-        <v>96.120866666666672</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84.365681818181798</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>41913</v>
       </c>
@@ -1968,10 +1974,10 @@
         <v>87.43</v>
       </c>
       <c r="D109" s="4">
-        <v>97.439604545454571</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85.680652173913046</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>41944</v>
       </c>
@@ -1982,10 +1988,10 @@
         <v>79.44</v>
       </c>
       <c r="D110" s="4">
-        <v>99.114688888888907</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>87.722149999999985</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>41974</v>
       </c>
@@ -1996,10 +2002,10 @@
         <v>62.34</v>
       </c>
       <c r="D111" s="4">
-        <v>101.44413333333333</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89.191913043478266</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>42005</v>
       </c>
@@ -2010,10 +2016,10 @@
         <v>47.76</v>
       </c>
       <c r="D112" s="4">
-        <v>103.76074000000001</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92.815045454545441</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>42036</v>
       </c>
@@ -2024,10 +2030,10 @@
         <v>58.1</v>
       </c>
       <c r="D113" s="4">
-        <v>105.16853888888889</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94.454599999999985</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>42064</v>
       </c>
@@ -2038,10 +2044,10 @@
         <v>55.89</v>
       </c>
       <c r="D114" s="4">
-        <v>107.36473809523811</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.897318181818179</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>42095</v>
       </c>
@@ -2052,10 +2058,10 @@
         <v>59.52</v>
       </c>
       <c r="D115" s="4">
-        <v>106.35228181818182</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.519363636363636</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>42125</v>
       </c>
@@ -2066,10 +2072,10 @@
         <v>64.08</v>
       </c>
       <c r="D116" s="4">
-        <v>105.40651499999998</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.237142857142842</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>42156</v>
       </c>
@@ -2080,10 +2086,10 @@
         <v>61.48</v>
       </c>
       <c r="D117" s="4">
-        <v>106.17898636363634</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.168590909090895</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>42186</v>
       </c>
@@ -2094,10 +2100,10 @@
         <v>56.56</v>
       </c>
       <c r="D118" s="4">
-        <v>108.12356818181816</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.925260869565193</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>42217</v>
       </c>
@@ -2108,10 +2114,10 @@
         <v>46.52</v>
       </c>
       <c r="D119" s="4">
-        <v>109.97674761904761</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.388095238095232</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>42248</v>
       </c>
@@ -2122,10 +2128,10 @@
         <v>47.62</v>
       </c>
       <c r="D120" s="4">
-        <v>110.85125714285715</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.814590909090924</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>42278</v>
       </c>
@@ -2136,10 +2142,10 @@
         <v>48.43</v>
       </c>
       <c r="D121" s="4">
-        <v>109.90357142857144</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.718363636363634</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>42309</v>
       </c>
@@ -2150,10 +2156,10 @@
         <v>44.27</v>
       </c>
       <c r="D122" s="4">
-        <v>111.6916105263158</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99.069571428571464</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>42339</v>
       </c>
@@ -2164,10 +2170,10 @@
         <v>38.01</v>
       </c>
       <c r="D123" s="4">
-        <v>112.7857409090909</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.314347826086959</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>42370</v>
       </c>
@@ -2178,10 +2184,10 @@
         <v>30.7</v>
       </c>
       <c r="D124" s="4">
-        <v>115.23438750000003</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.996523809523794</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>42401</v>
       </c>
@@ -2192,10 +2198,10 @@
         <v>32.18</v>
       </c>
       <c r="D125" s="4">
-        <v>114.28173499999998</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.040761904761894</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>42430</v>
       </c>
@@ -2206,10 +2212,10 @@
         <v>38.21</v>
       </c>
       <c r="D126" s="4">
-        <v>111.89339130434782</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.259913043478264</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>42461</v>
       </c>
@@ -2220,10 +2226,10 @@
         <v>41.58</v>
       </c>
       <c r="D127" s="4">
-        <v>110.01707619047619</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94.40361904761906</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>42491</v>
       </c>
@@ -2234,10 +2240,10 @@
         <v>46.74</v>
       </c>
       <c r="D128" s="4">
-        <v>111.14051428571426</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94.567909090909083</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>42522</v>
       </c>
@@ -2248,10 +2254,10 @@
         <v>48.25</v>
       </c>
       <c r="D129" s="4">
-        <v>111.5596272727273</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94.635565217391317</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>42552</v>
       </c>
@@ -2262,10 +2268,10 @@
         <v>44.95</v>
       </c>
       <c r="D130" s="4">
-        <v>112.47729</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.528095238095247</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>42583</v>
       </c>
@@ -2276,10 +2282,10 @@
         <v>45.84</v>
       </c>
       <c r="D131" s="4">
-        <v>111.43836956521741</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.38039130434781</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>42614</v>
       </c>
@@ -2290,10 +2296,10 @@
         <v>46.57</v>
       </c>
       <c r="D132" s="4">
-        <v>112.31686190476191</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.479090909090928</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>42644</v>
       </c>
@@ -2304,10 +2310,10 @@
         <v>49.52</v>
       </c>
       <c r="D133" s="4">
-        <v>113.47469499999997</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.714476190476191</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>42675</v>
       </c>
@@ -2318,10 +2324,10 @@
         <v>44.73</v>
       </c>
       <c r="D134" s="4">
-        <v>116.10751500000001</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99.768181818181816</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <v>42705</v>
       </c>
@@ -2332,10 +2338,10 @@
         <v>53.31</v>
       </c>
       <c r="D135" s="4">
-        <v>117.90482857142855</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102.04136363636363</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>42736</v>
       </c>
@@ -2346,10 +2352,10 @@
         <v>54.58</v>
       </c>
       <c r="D136" s="4">
-        <v>117.78607894736845</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+        <v>101.20236363636364</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>42767</v>
       </c>
@@ -2360,10 +2366,10 @@
         <v>54.87</v>
       </c>
       <c r="D137" s="4">
-        <v>116.12033684210526</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100.6953</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>42795</v>
       </c>
@@ -2374,10 +2380,10 @@
         <v>51.59</v>
       </c>
       <c r="D138" s="4">
-        <v>115.65538260869566</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100.75969565217389</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>42826</v>
       </c>
@@ -2388,10 +2394,10 @@
         <v>52.31</v>
       </c>
       <c r="D139" s="4">
-        <v>114.76978500000003</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100.07250000000002</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <v>42856</v>
       </c>
@@ -2402,10 +2408,10 @@
         <v>50.33</v>
       </c>
       <c r="D140" s="4">
-        <v>114.26073181818184</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.238608695652189</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>42887</v>
       </c>
@@ -2416,10 +2422,10 @@
         <v>46.37</v>
       </c>
       <c r="D141" s="4">
-        <v>112.76137272727274</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.943045454545441</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <v>42917</v>
       </c>
@@ -2430,10 +2436,10 @@
         <v>48.48</v>
       </c>
       <c r="D142" s="4">
-        <v>111.06173500000003</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94.915857142857149</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>42948</v>
       </c>
@@ -2444,10 +2450,10 @@
         <v>51.7</v>
       </c>
       <c r="D143" s="4">
-        <v>109.90734782608695</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93.175217391304358</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>42979</v>
       </c>
@@ -2458,10 +2464,10 @@
         <v>56.15</v>
       </c>
       <c r="D144" s="4">
-        <v>108.85588500000001</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92.373681818181822</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>43009</v>
       </c>
@@ -2472,10 +2478,10 @@
         <v>57.51</v>
       </c>
       <c r="D145" s="4">
-        <v>110.89130476190478</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93.708227272727285</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>43040</v>
       </c>
@@ -2486,10 +2492,10 @@
         <v>62.71</v>
       </c>
       <c r="D146" s="4">
-        <v>111.165785</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93.962499999999991</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
         <v>43070</v>
       </c>
@@ -2500,10 +2506,10 @@
         <v>64.37</v>
       </c>
       <c r="D147" s="4">
-        <v>110.87863</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93.381142857142876</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>43101</v>
       </c>
@@ -2514,10 +2520,10 @@
         <v>69.08</v>
       </c>
       <c r="D148" s="4">
-        <v>108.36004761904762</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.816173913043471</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>43132</v>
       </c>
@@ -2528,10 +2534,10 @@
         <v>65.319999999999993</v>
       </c>
       <c r="D149" s="4">
-        <v>107.65337368421052</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89.695599999999985</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>43160</v>
       </c>
@@ -2542,10 +2548,10 @@
         <v>66.02</v>
       </c>
       <c r="D150" s="4">
-        <v>107.950605</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89.877272727272725</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>43191</v>
       </c>
@@ -2556,10 +2562,10 @@
         <v>72.11</v>
       </c>
       <c r="D151" s="4">
-        <v>107.94613809523811</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.349818181818165</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>43221</v>
       </c>
@@ -2570,10 +2576,10 @@
         <v>76.98</v>
       </c>
       <c r="D152" s="4">
-        <v>111.04937727272726</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93.336304347826086</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>43252</v>
       </c>
@@ -2584,10 +2590,10 @@
         <v>74.41</v>
       </c>
       <c r="D153" s="4">
-        <v>112.84701904761906</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94.333909090909117</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>43282</v>
       </c>
@@ -2598,10 +2604,10 @@
         <v>74.25</v>
       </c>
       <c r="D154" s="4">
-        <v>113.06286666666668</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94.609590909090912</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
         <v>43313</v>
       </c>
@@ -2612,10 +2618,10 @@
         <v>72.53</v>
       </c>
       <c r="D155" s="4">
-        <v>113.83435217391306</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.48047826086956</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>43344</v>
       </c>
@@ -2626,10 +2632,10 @@
         <v>78.89</v>
       </c>
       <c r="D156" s="4">
-        <v>114.08177368421052</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94.756700000000023</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <v>43374</v>
       </c>
@@ -2640,10 +2646,10 @@
         <v>81.03</v>
       </c>
       <c r="D157" s="4">
-        <v>114.83369090909088</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.851086956521726</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>43405</v>
       </c>
@@ -2654,10 +2660,10 @@
         <v>64.75</v>
       </c>
       <c r="D158" s="4">
-        <v>116.17139999999999</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.760409090909079</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <v>43435</v>
       </c>
@@ -2668,10 +2674,10 @@
         <v>57.36</v>
       </c>
       <c r="D159" s="4">
-        <v>116.21466842105261</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.852086956521731</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>43466</v>
       </c>
@@ -2682,10 +2688,10 @@
         <v>59.41</v>
       </c>
       <c r="D160" s="4">
-        <v>114.44390000000001</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.966260869565218</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <v>43497</v>
       </c>
@@ -2696,10 +2702,10 @@
         <v>63.96</v>
       </c>
       <c r="D161" s="4">
-        <v>114.41411111111113</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.477761904761905</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
         <v>43525</v>
       </c>
@@ -2710,10 +2716,10 @@
         <v>66.14</v>
       </c>
       <c r="D162" s="4">
-        <v>114.7857619047619</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.779857142857168</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
         <v>43556</v>
       </c>
@@ -2724,10 +2730,10 @@
         <v>71.23</v>
       </c>
       <c r="D163" s="4">
-        <v>114.90592727272728</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.364772727272737</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
         <v>43586</v>
       </c>
@@ -2738,10 +2744,10 @@
         <v>71.319999999999993</v>
       </c>
       <c r="D164" s="4">
-        <v>115.96051818181817</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.733782608695648</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
         <v>43617</v>
       </c>
@@ -2752,10 +2758,10 @@
         <v>64.22</v>
       </c>
       <c r="D165" s="4">
-        <v>115.43132499999999</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.799000000000007</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <v>43647</v>
       </c>
@@ -2766,10 +2772,10 @@
         <v>63.92</v>
       </c>
       <c r="D166" s="4">
-        <v>115.08204545454547</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.341478260869579</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
         <v>43678</v>
       </c>
@@ -2780,10 +2786,10 @@
         <v>59.04</v>
       </c>
       <c r="D167" s="4">
-        <v>117.10523181818185</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.003090909090915</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <v>43709</v>
       </c>
@@ -2794,10 +2800,10 @@
         <v>62.83</v>
       </c>
       <c r="D168" s="4">
-        <v>117.32881499999999</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.6095714285714</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <v>43739</v>
       </c>
@@ -2808,10 +2814,10 @@
         <v>59.71</v>
       </c>
       <c r="D169" s="4">
-        <v>116.75106363636364</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.19745833333333</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
         <v>43770</v>
       </c>
@@ -2822,10 +2828,10 @@
         <v>63.21</v>
       </c>
       <c r="D170" s="4">
-        <v>116.56367368421056</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.078761904761905</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
         <v>43800</v>
       </c>
@@ -2836,10 +2842,10 @@
         <v>67.31</v>
       </c>
       <c r="D171" s="4">
-        <v>115.91388500000001</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.377863636363642</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <v>43831</v>
       </c>
@@ -2850,10 +2856,10 @@
         <v>63.65</v>
       </c>
       <c r="D172" s="4">
-        <v>115.28190476190478</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.399521739130435</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="2">
         <v>43862</v>
       </c>
@@ -2864,10 +2870,10 @@
         <v>55.66</v>
       </c>
       <c r="D173" s="4">
-        <v>116.71380526315788</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.876047619047611</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <v>43891</v>
       </c>
@@ -2878,10 +2884,10 @@
         <v>32.01</v>
       </c>
       <c r="D174" s="4">
-        <v>121.02455454545454</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.84322727272729</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="2">
         <v>43922</v>
       </c>
@@ -2892,10 +2898,10 @@
         <v>18.38</v>
       </c>
       <c r="D175" s="4">
-        <v>123.28346818181818</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99.889590909090899</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <v>43952</v>
       </c>
@@ -2906,10 +2912,10 @@
         <v>29.38</v>
       </c>
       <c r="D176" s="4">
-        <v>122.61873500000004</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99.581809523809511</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="2">
         <v>43983</v>
       </c>
@@ -2920,10 +2926,10 @@
         <v>40.270000000000003</v>
       </c>
       <c r="D177" s="4">
-        <v>119.68094090909089</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.106826086956517</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <v>44013</v>
       </c>
@@ -2934,10 +2940,10 @@
         <v>43.24</v>
       </c>
       <c r="D178" s="4">
-        <v>118.69559545454545</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.583217391304359</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>44044</v>
       </c>
@@ -2948,10 +2954,10 @@
         <v>44.74</v>
       </c>
       <c r="D179" s="4">
-        <v>116.95257142857145</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93.046999999999997</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>44075</v>
       </c>
@@ -2962,10 +2968,10 @@
         <v>40.909999999999997</v>
       </c>
       <c r="D180" s="4">
-        <v>116.34884761904762</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93.463869565217379</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <v>44105</v>
       </c>
@@ -2976,10 +2982,10 @@
         <v>40.19</v>
       </c>
       <c r="D181" s="4">
-        <v>115.78389523809525</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93.398590909090913</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>44136</v>
       </c>
@@ -2990,10 +2996,10 @@
         <v>42.69</v>
       </c>
       <c r="D182" s="4">
-        <v>114.09983333333334</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92.595999999999989</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <v>44166</v>
       </c>
@@ -3004,10 +3010,10 @@
         <v>49.99</v>
       </c>
       <c r="D183" s="4">
-        <v>111.90164285714285</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.507217391304351</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>44197</v>
       </c>
@@ -3018,10 +3024,10 @@
         <v>54.77</v>
       </c>
       <c r="D184" s="4">
-        <v>111.49137777777779</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.236857142857147</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <v>44228</v>
       </c>
@@ -3032,10 +3038,10 @@
         <v>62.28</v>
       </c>
       <c r="D185" s="4">
-        <v>112.02478947368421</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.628</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>44256</v>
       </c>
@@ -3046,10 +3052,10 @@
         <v>65.41</v>
       </c>
       <c r="D186" s="4">
-        <v>113.34895217391305</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91.994173913043483</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <v>44287</v>
       </c>
@@ -3060,10 +3066,10 @@
         <v>64.81</v>
       </c>
       <c r="D187" s="4">
-        <v>112.64088181818182</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91.618217391304356</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>44317</v>
       </c>
@@ -3074,10 +3080,10 @@
         <v>68.53</v>
       </c>
       <c r="D188" s="4">
-        <v>111.22630999999998</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.30247619047617</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <v>44348</v>
       </c>
@@ -3088,10 +3094,10 @@
         <v>73.16</v>
       </c>
       <c r="D189" s="4">
-        <v>111.58851363636367</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91.043590909090881</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>44378</v>
       </c>
@@ -3102,10 +3108,10 @@
         <v>75.17</v>
       </c>
       <c r="D190" s="4">
-        <v>113.06898095238095</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92.513590909090908</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>44409</v>
       </c>
@@ -3116,10 +3122,10 @@
         <v>70.75</v>
       </c>
       <c r="D191" s="4">
-        <v>113.40918636363639</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92.79904545454545</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>44440</v>
       </c>
@@ -3130,10 +3136,10 @@
         <v>74.489999999999995</v>
       </c>
       <c r="D192" s="4">
-        <v>113.44822857142856</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92.93669565217391</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="2">
         <v>44470</v>
       </c>
@@ -3144,10 +3150,10 @@
         <v>83.54</v>
       </c>
       <c r="D193" s="4">
-        <v>114.07398000000001</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93.944285714285712</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <v>44501</v>
       </c>
@@ -3158,10 +3164,10 @@
         <v>81.05</v>
       </c>
       <c r="D194" s="4">
-        <v>115.001565</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.340772727272721</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="2">
         <v>44531</v>
       </c>
@@ -3172,10 +3178,10 @@
         <v>74.17</v>
       </c>
       <c r="D195" s="4">
-        <v>115.81335714285717</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.199217391304344</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="2">
         <v>44562</v>
       </c>
@@ -3186,10 +3192,10 @@
         <v>86.51</v>
       </c>
       <c r="D196" s="4">
-        <v>115.04962499999999</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.909545454545466</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="2">
         <v>44593</v>
       </c>
@@ -3200,10 +3206,10 @@
         <v>97.13</v>
       </c>
       <c r="D197" s="4">
-        <v>115.01305263157894</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96.000749999999996</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>44621</v>
       </c>
@@ -3214,10 +3220,10 @@
         <v>117.25</v>
       </c>
       <c r="D198" s="4">
-        <v>116.36742173913044</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.473565217391283</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <v>44652</v>
       </c>
@@ -3228,10 +3234,10 @@
         <v>104.58</v>
       </c>
       <c r="D199" s="4">
-        <v>117.17941428571427</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100.69104761904762</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>44682</v>
       </c>
@@ -3242,10 +3248,10 @@
         <v>113.34</v>
       </c>
       <c r="D200" s="4">
-        <v>119.66495714285713</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103.09890909090909</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="2">
         <v>44713</v>
       </c>
@@ -3256,10 +3262,10 @@
         <v>122.71</v>
       </c>
       <c r="D201" s="4">
-        <v>119.96283809523811</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103.88177272727272</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <v>44743</v>
       </c>
@@ -3270,10 +3276,10 @@
         <v>111.93</v>
       </c>
       <c r="D202" s="4">
-        <v>122.648325</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+        <v>106.94490476190478</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
         <v>44774</v>
       </c>
@@ -3284,10 +3290,10 @@
         <v>100.45</v>
       </c>
       <c r="D203" s="4">
-        <v>122.23727826086956</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+        <v>107.14947826086957</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <v>44805</v>
       </c>
@@ -3298,10 +3304,10 @@
         <v>89.76</v>
       </c>
       <c r="D204" s="4">
-        <v>125.50693333333332</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+        <v>110.702</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="2">
         <v>44835</v>
       </c>
@@ -3312,10 +3318,10 @@
         <v>93.33</v>
       </c>
       <c r="D205" s="4">
-        <v>127.40840499999999</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+        <v>111.94509523809525</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="2">
         <v>44866</v>
       </c>
@@ -3326,10 +3332,10 @@
         <v>91.42</v>
       </c>
       <c r="D206" s="4">
-        <v>124.81488500000003</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+        <v>108.0349090909091</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="2">
         <v>44896</v>
       </c>
@@ -3340,10 +3346,10 @@
         <v>80.92</v>
       </c>
       <c r="D207" s="4">
-        <v>122.20212857142856</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+        <v>104.49422727272727</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="2">
         <v>44927</v>
       </c>
@@ -3354,10 +3360,10 @@
         <v>82.5</v>
       </c>
       <c r="D208" s="4">
-        <v>119.77648499999998</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102.77784782608695</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <v>44958</v>
       </c>
@@ -3368,10 +3374,10 @@
         <v>82.59</v>
       </c>
       <c r="D209" s="4">
-        <v>120.31560526315791</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103.67828571428572</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="2">
         <v>44986</v>
       </c>
@@ -3382,10 +3388,10 @@
         <v>78.430000000000007</v>
       </c>
       <c r="D210" s="4">
-        <v>120.80600434782612</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103.73862499999997</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="2">
         <v>45017</v>
       </c>
@@ -3396,10 +3402,10 @@
         <v>84.64</v>
       </c>
       <c r="D211" s="4">
-        <v>119.41827999999998</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+        <v>101.78040000000001</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="2">
         <v>45047</v>
       </c>
@@ -3410,35 +3416,175 @@
         <v>75.47</v>
       </c>
       <c r="D212" s="4">
-        <v>119.8552090909091</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102.77000000000002</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="2">
         <v>45078</v>
       </c>
       <c r="B213" s="3">
-        <v>4233.9459999999999</v>
+        <v>4191.677391304348</v>
       </c>
       <c r="C213" s="4">
         <v>74.84</v>
       </c>
       <c r="D213" s="4">
-        <v>119.71037142857142</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103.04378260869565</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="2">
         <v>45108</v>
       </c>
       <c r="B214" s="3">
-        <v>4163.5028571428575</v>
+        <v>4048.2304761904761</v>
       </c>
       <c r="C214" s="4">
-        <v>79.39</v>
+        <v>80.11</v>
       </c>
       <c r="D214" s="4">
-        <v>119.88460000000001</v>
+        <v>101.40315238095238</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" s="2">
+        <v>45139</v>
+      </c>
+      <c r="B215" s="3">
+        <v>4073.9391304347828</v>
+      </c>
+      <c r="C215" s="4">
+        <v>86.15</v>
+      </c>
+      <c r="D215" s="4">
+        <v>103.10286956521743</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" s="2">
+        <v>45170</v>
+      </c>
+      <c r="B216" s="3">
+        <v>4005.7181818181812</v>
+      </c>
+      <c r="C216" s="4">
+        <v>93.72</v>
+      </c>
+      <c r="D216" s="4">
+        <v>105.29150000000003</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" s="2">
+        <v>45200</v>
+      </c>
+      <c r="B217" s="3">
+        <v>4217.8736363636363</v>
+      </c>
+      <c r="C217" s="4">
+        <v>90.6</v>
+      </c>
+      <c r="D217" s="4">
+        <v>106.35481818181819</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" s="2">
+        <v>45231</v>
+      </c>
+      <c r="B218" s="3">
+        <v>4026.5904545454546</v>
+      </c>
+      <c r="C218" s="4">
+        <v>82.94</v>
+      </c>
+      <c r="D218" s="4">
+        <v>104.49</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" s="2">
+        <v>45261</v>
+      </c>
+      <c r="B219" s="3">
+        <v>3964.72</v>
+      </c>
+      <c r="C219" s="4">
+        <v>77.63</v>
+      </c>
+      <c r="D219" s="4">
+        <v>102.64</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" s="2">
+        <v>45292</v>
+      </c>
+      <c r="B220" s="3">
+        <v>3915.336956521739</v>
+      </c>
+      <c r="C220" s="4">
+        <v>80.12</v>
+      </c>
+      <c r="D220" s="4">
+        <v>102.88</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" s="2">
+        <v>45323</v>
+      </c>
+      <c r="B221" s="3">
+        <v>3926.6786363636361</v>
+      </c>
+      <c r="C221" s="4">
+        <v>83.48</v>
+      </c>
+      <c r="D221" s="4">
+        <v>104.13</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" s="2">
+        <v>45352</v>
+      </c>
+      <c r="B222" s="3">
+        <v>3895.5733333333328</v>
+      </c>
+      <c r="C222" s="4">
+        <v>85.41</v>
+      </c>
+      <c r="D222" s="4">
+        <v>103.67</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B223" s="3">
+        <v>3862.4481818181816</v>
+      </c>
+      <c r="C223" s="4">
+        <v>89.94</v>
+      </c>
+      <c r="D223" s="4">
+        <v>105.41</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" s="2">
+        <v>45413</v>
+      </c>
+      <c r="B224" s="3">
+        <v>3863.3773913043483</v>
+      </c>
+      <c r="C224" s="4">
+        <v>81.75</v>
+      </c>
+      <c r="D224" s="4">
+        <v>104.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>